<commit_message>
Unpolished but functional output
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -8,53 +8,133 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tbryant\Repos\AKL-cleaning-roster-updated\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{190D26E2-B5DC-4A7D-A019-F411A9EDEF52}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDDF2CC-D283-490E-B969-203FFC531AA4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{1608D09D-738C-4CA7-9448-A6B0834C8F3A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>this</t>
-  </si>
-  <si>
-    <t>is</t>
-  </si>
-  <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>data</t>
-  </si>
-  <si>
-    <t>frame</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="36">
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>First Floor Bathroom</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Second Floor Bathroom</t>
+  </si>
+  <si>
+    <t>Sanitize</t>
+  </si>
+  <si>
+    <t>Parker</t>
+  </si>
+  <si>
+    <t>Kitchen</t>
+  </si>
+  <si>
+    <t>Trash</t>
+  </si>
+  <si>
+    <t>Attic</t>
+  </si>
+  <si>
+    <t>Tommy</t>
+  </si>
+  <si>
+    <t>Eagles Nest</t>
+  </si>
+  <si>
+    <t>Chapter Room</t>
+  </si>
+  <si>
+    <t>Odd Jobs</t>
+  </si>
+  <si>
+    <t>No Job</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>First Floor Sweep</t>
+  </si>
+  <si>
+    <t>First Floor Swiffer</t>
+  </si>
+  <si>
+    <t>Second Floor Sweep</t>
+  </si>
+  <si>
+    <t>Second Floor Swiffer</t>
+  </si>
+  <si>
+    <t>Laundry Room</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Week 4</t>
+  </si>
+  <si>
+    <t>Person 1</t>
+  </si>
+  <si>
+    <t>Person 2</t>
+  </si>
+  <si>
+    <t>Person 3</t>
+  </si>
+  <si>
+    <t>Person 4</t>
+  </si>
+  <si>
+    <t>Person 5</t>
+  </si>
+  <si>
+    <t>Week1</t>
+  </si>
+  <si>
+    <t>Week2</t>
+  </si>
+  <si>
+    <t>Week3</t>
+  </si>
+  <si>
+    <t>Week4</t>
+  </si>
+  <si>
+    <t>kitchen</t>
+  </si>
+  <si>
+    <t>bathroom</t>
+  </si>
+  <si>
+    <t>laundry</t>
+  </si>
+  <si>
+    <t>etc</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,13 +142,33 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -83,8 +183,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -398,36 +501,445 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EEF180C5-3E6E-4F35-A13D-43ECA37AEE1B}">
-  <dimension ref="A1:F1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K1" t="s">
+        <v>29</v>
+      </c>
+      <c r="L1" t="s">
+        <v>30</v>
+      </c>
+      <c r="M1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1">
+      <c r="I2" t="s">
+        <v>2</v>
+      </c>
+      <c r="J2" t="s">
+        <v>32</v>
+      </c>
+      <c r="K2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L2" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="I3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="I5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B21" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B23" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
         <v>4</v>
+      </c>
+      <c r="B38" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A41" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A42" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A43" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A44" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A45" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A46" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B46" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A47" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B53" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B60" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B61" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A65" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A66" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A67" s="2" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned old comments up, removed temp work files
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="10" yWindow="10" windowWidth="19180" windowHeight="10780" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="output" sheetId="1" state="visible" r:id="rId1"/>
@@ -447,10 +447,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F67"/>
+  <dimension ref="A1:F59"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D62" sqref="D62"/>
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="14.5"/>
@@ -538,157 +538,177 @@
           <t>Jwags</t>
         </is>
       </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Sidney</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Tryce</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Sanitize</t>
+          <t>Kitchen</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Jwags</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Jaxson</t>
+          <t>Landon</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>Goode</t>
+          <t>Aaron</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>Peyton</t>
+          <t>Jerzey</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Jaxson</t>
+          <t>Schofield</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Kitchen</t>
+          <t>Trash</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Jwags</t>
+          <t>Riley</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Landon</t>
+          <t>Creason</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>Tryce</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>Aaron</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Jerzey</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>Tryce</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Trash</t>
+          <t>Attic</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Riley</t>
+          <t>Tommy</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Creason</t>
+          <t>Kaleb</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>EvanV</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>Tryce</t>
+          <t>Hernandez</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Sam</t>
+          <t>Garrett</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Attic</t>
+          <t>Eagles Nest</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Tommy</t>
+          <t>Jerzey</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Kaleb</t>
+          <t>Ben</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>EvanV</t>
+          <t>Goode</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Hurley</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Noah</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Eagles Nest</t>
+          <t>Chapter Room</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Jerzey</t>
+          <t>Tanner</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Schofield</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>Goode</t>
+          <t>Brayden</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
+        <is>
+          <t>Hurley</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
         <is>
           <t>Hurley</t>
         </is>
@@ -697,221 +717,337 @@
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Chapter Room</t>
+          <t>Odd Jobs</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Tanner</t>
+          <t>Nathan</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Schofield</t>
+          <t>Sidney</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>Brayden</t>
+          <t>Sam</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Hurley</t>
+          <t>Noah</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Riley</t>
+          <t>Jaxson</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Odd Jobs</t>
+          <t>No Job</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Nathan</t>
+          <t>Noah</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Sidney</t>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>Jwags</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>Mason</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Jerzey</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>No Job</t>
+          <t>First Floor Sweep</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Noah</t>
+          <t>Trey</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Tommy</t>
+          <t>Schofield</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>Kaleb</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Kaleb</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2" t="inlineStr">
         <is>
-          <t>First Floor Sweep</t>
+          <t>First Floor Swiffer</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
           <t>Trey</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Schofield</t>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>Sidney</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Tommy</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2" t="inlineStr">
         <is>
-          <t>First Floor Swiffer</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Mike</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Trey</t>
+          <t>Second Floor Sweep</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2" t="inlineStr">
         <is>
-          <t>Second Floor Sweep</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
           <t>Second Floor Swiffer</t>
         </is>
       </c>
     </row>
+    <row r="15"/>
     <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Laundry Room</t>
+      <c r="A16" s="1" t="inlineStr">
+        <is>
+          <t>Week 2</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>First Floor Bathroom</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Jerzey</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Sidney</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Brayden</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>EvanV</t>
         </is>
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="1" t="inlineStr">
-        <is>
-          <t>Week 2</t>
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Second Floor Bathroom</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Jerzey</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Garrett</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2" t="inlineStr">
         <is>
-          <t>First Floor Bathroom</t>
+          <t>Kitchen</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Tommy</t>
+          <t>Sidney</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Jerzey</t>
+          <t>Mason</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Sidney</t>
+          <t>Kaleb</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Brayden</t>
+          <t>Trey</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Hurley</t>
+          <t>Tryce</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2" t="inlineStr">
         <is>
-          <t>Second Floor Bathroom</t>
+          <t>Trash</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>Goode</t>
+        </is>
+      </c>
+      <c r="D20" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>Jerzey</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Blake</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="2" t="inlineStr">
         <is>
-          <t>Sanitize</t>
+          <t>Attic</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Jwags</t>
+          <t>Trey</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Tanner</t>
+          <t>Nathan</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>Schofield</t>
+          <t>Riley</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Landon</t>
+          <t>Sam</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Tryce</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="2" t="inlineStr">
         <is>
-          <t>Kitchen</t>
+          <t>Eagles Nest</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>Sidney</t>
+          <t>Mason</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Mason</t>
+          <t>Hernandez</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>Kaleb</t>
+          <t>Creason</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Trey</t>
+          <t>Tommy</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
@@ -923,263 +1059,303 @@
     <row r="23">
       <c r="A23" s="2" t="inlineStr">
         <is>
-          <t>Trash</t>
+          <t>Chapter Room</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>Mike</t>
+          <t>Noah</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Goode</t>
+          <t>Kaleb</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Jaxson</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Jerzey</t>
+          <t>EvanV</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Trey</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2" t="inlineStr">
         <is>
-          <t>Attic</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Trey</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>Nathan</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>Riley</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>Sam</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Tryce</t>
+          <t>Odd Jobs</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2" t="inlineStr">
         <is>
-          <t>Eagles Nest</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Mason</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>Hernandez</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>Creason</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>Tommy</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Landon</t>
+          <t>No Job</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2" t="inlineStr">
         <is>
-          <t>Chapter Room</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Noah</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Kaleb</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Jaxson</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>EvanV</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Blake</t>
+          <t>First Floor Sweep</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2" t="inlineStr">
         <is>
-          <t>Odd Jobs</t>
+          <t>First Floor Swiffer</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2" t="inlineStr">
         <is>
-          <t>No Job</t>
+          <t>Second Floor Sweep</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2" t="inlineStr">
         <is>
-          <t>First Floor Sweep</t>
+          <t>Second Floor Swiffer</t>
         </is>
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="2" t="inlineStr">
-        <is>
-          <t>First Floor Swiffer</t>
-        </is>
-      </c>
+      <c r="A30" s="2" t="n"/>
     </row>
     <row r="31">
-      <c r="A31" s="2" t="inlineStr">
-        <is>
-          <t>Second Floor Sweep</t>
+      <c r="A31" s="1" t="inlineStr">
+        <is>
+          <t>Week 3</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2" t="inlineStr">
         <is>
-          <t>Second Floor Swiffer</t>
+          <t>First Floor Bathroom</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Jwags</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Hernandez</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Aaron</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2" t="inlineStr">
         <is>
-          <t>Laundry Room</t>
+          <t>Second Floor Bathroom</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Tryce</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Blake</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>Sidney</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Hurley</t>
         </is>
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="2" t="n"/>
+      <c r="A34" s="2" t="inlineStr">
+        <is>
+          <t>Kitchen</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Jwags</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Hernandez</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>Jaxson</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Hurley</t>
+        </is>
+      </c>
     </row>
     <row r="35">
-      <c r="A35" s="1" t="inlineStr">
-        <is>
-          <t>Week 3</t>
+      <c r="A35" s="2" t="inlineStr">
+        <is>
+          <t>Trash</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Mason</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Tanner</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Peyton</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2" t="inlineStr">
         <is>
-          <t>First Floor Bathroom</t>
+          <t>Attic</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>Jwags</t>
+          <t>Jaxson</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Hernandez</t>
+          <t>Creason</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Brayden</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>Noah</t>
+          <t>Landon</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Ben</t>
+          <t>Blake</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2" t="inlineStr">
         <is>
-          <t>Second Floor Bathroom</t>
+          <t>Eagles Nest</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>Tryce</t>
+          <t>Garrett</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Blake</t>
+          <t>Hurley</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Jerzey</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Kaleb</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Garrett</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2" t="inlineStr">
         <is>
-          <t>Sanitize</t>
+          <t>Chapter Room</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>Tommy</t>
+          <t>Jerzey</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Kaleb</t>
+          <t>Sidney</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>Trey</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Riley</t>
+          <t>Goode</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
@@ -1191,499 +1367,318 @@
     <row r="39">
       <c r="A39" s="2" t="inlineStr">
         <is>
-          <t>Kitchen</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>Tommy</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Jwags</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Hernandez</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Jaxson</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>Landon</t>
+          <t>Odd Jobs</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2" t="inlineStr">
         <is>
-          <t>Trash</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Noah</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Mason</t>
-        </is>
-      </c>
-      <c r="D40" t="inlineStr">
-        <is>
-          <t>Tanner</t>
-        </is>
-      </c>
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>Nathan</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>Garrett</t>
+          <t>No Job</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="2" t="inlineStr">
         <is>
-          <t>Attic</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>Jaxson</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Creason</t>
-        </is>
-      </c>
-      <c r="D41" t="inlineStr">
-        <is>
-          <t>Brayden</t>
-        </is>
-      </c>
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>Landon</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Mike</t>
+          <t>First Floor Sweep</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" s="2" t="inlineStr">
         <is>
-          <t>Eagles Nest</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Garrett</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Hurley</t>
-        </is>
-      </c>
-      <c r="D42" t="inlineStr">
-        <is>
-          <t>Jerzey</t>
-        </is>
-      </c>
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>Kaleb</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>Aaron</t>
+          <t>First Floor Swiffer</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" s="2" t="inlineStr">
         <is>
-          <t>Chapter Room</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>Jerzey</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>Sidney</t>
-        </is>
-      </c>
-      <c r="D43" t="inlineStr">
-        <is>
-          <t>Mike</t>
-        </is>
-      </c>
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>Goode</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>Hurley</t>
+          <t>Second Floor Sweep</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2" t="inlineStr">
         <is>
-          <t>Odd Jobs</t>
+          <t>Second Floor Swiffer</t>
         </is>
       </c>
     </row>
     <row r="45">
-      <c r="A45" s="2" t="inlineStr">
-        <is>
-          <t>No Job</t>
-        </is>
-      </c>
+      <c r="A45" s="2" t="n"/>
     </row>
     <row r="46">
-      <c r="A46" s="2" t="inlineStr">
-        <is>
-          <t>First Floor Sweep</t>
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>Week 4</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2" t="inlineStr">
         <is>
-          <t>First Floor Swiffer</t>
+          <t>First Floor Bathroom</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Noah</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Nathan</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Riley</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>Creason</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Tryce</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2" t="inlineStr">
         <is>
-          <t>Second Floor Sweep</t>
+          <t>Second Floor Bathroom</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Jerzey</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Riley</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Schofield</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Blake</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2" t="inlineStr">
         <is>
-          <t>Second Floor Swiffer</t>
+          <t>Kitchen</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Tanner</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Goode</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Peyton</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>EvanV</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2" t="inlineStr">
         <is>
-          <t>Laundry Room</t>
+          <t>Trash</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Kaleb</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Trey</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Jaxson</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Brayden</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Goode</t>
         </is>
       </c>
     </row>
     <row r="51">
-      <c r="A51" s="2" t="n"/>
+      <c r="A51" s="2" t="inlineStr">
+        <is>
+          <t>Attic</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Sidney</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Tanner</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Peyton</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>Kaleb</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Aaron</t>
+        </is>
+      </c>
     </row>
     <row r="52">
-      <c r="A52" s="1" t="inlineStr">
-        <is>
-          <t>Week 4</t>
+      <c r="A52" s="2" t="inlineStr">
+        <is>
+          <t>Eagles Nest</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Tommy</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Jwags</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Schofield</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Mike</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Landon</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2" t="inlineStr">
         <is>
-          <t>First Floor Bathroom</t>
+          <t>Chapter Room</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>Noah</t>
+          <t>Hernandez</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Nathan</t>
+          <t>Aaron</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
         <is>
-          <t>Riley</t>
+          <t>Sidney</t>
         </is>
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Creason</t>
+          <t>Mike</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Garrett</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2" t="inlineStr">
         <is>
-          <t>Second Floor Bathroom</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Tommy</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>Jerzey</t>
-        </is>
-      </c>
-      <c r="D54" t="inlineStr">
-        <is>
-          <t>Riley</t>
-        </is>
-      </c>
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>Schofield</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>Landon</t>
+          <t>Odd Jobs</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2" t="inlineStr">
         <is>
-          <t>Sanitize</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>Jerzey</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>Mason</t>
+          <t>No Job</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2" t="inlineStr">
         <is>
-          <t>Kitchen</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>Tanner</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>Goode</t>
-        </is>
-      </c>
-      <c r="D56" t="inlineStr">
-        <is>
-          <t>Peyton</t>
+          <t>First Floor Sweep</t>
         </is>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2" t="inlineStr">
         <is>
-          <t>Trash</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>Kaleb</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>Trey</t>
-        </is>
-      </c>
-      <c r="D57" t="inlineStr">
-        <is>
-          <t>Jaxson</t>
-        </is>
-      </c>
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>Brayden</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>Tryce</t>
+          <t>First Floor Swiffer</t>
         </is>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2" t="inlineStr">
         <is>
-          <t>Attic</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>Sidney</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>Tanner</t>
-        </is>
-      </c>
-      <c r="D58" t="inlineStr">
-        <is>
-          <t>Peyton</t>
-        </is>
-      </c>
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>Kaleb</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>Hurley</t>
+          <t>Second Floor Sweep</t>
         </is>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2" t="inlineStr">
         <is>
-          <t>Eagles Nest</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>Tommy</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>Jwags</t>
-        </is>
-      </c>
-      <c r="D59" t="inlineStr">
-        <is>
-          <t>Schofield</t>
-        </is>
-      </c>
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>Mike</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>Blake</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" s="2" t="inlineStr">
-        <is>
-          <t>Chapter Room</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>Hernandez</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>Aaron</t>
-        </is>
-      </c>
-      <c r="D60" t="inlineStr">
-        <is>
-          <t>Sidney</t>
-        </is>
-      </c>
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>Mike</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>Garrett</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" s="2" t="inlineStr">
-        <is>
-          <t>Odd Jobs</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" s="2" t="inlineStr">
-        <is>
-          <t>No Job</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" s="2" t="inlineStr">
-        <is>
-          <t>First Floor Sweep</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" s="2" t="inlineStr">
-        <is>
-          <t>First Floor Swiffer</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" s="2" t="inlineStr">
-        <is>
-          <t>Second Floor Sweep</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" s="2" t="inlineStr">
-        <is>
           <t>Second Floor Swiffer</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" s="2" t="inlineStr">
-        <is>
-          <t>Laundry Room</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Commented Thoughts on How to Improve This Old-ish Program
Been a while since I've looked at this project. It's quite a bit ugly and inneficient compared to what I remember it being. I would start from scratch if I felt the need to re-code this. Commented are my thoughts on what to do differently
</commit_message>
<xml_diff>
--- a/test_output.xlsx
+++ b/test_output.xlsx
@@ -518,7 +518,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>Blake</t>
+          <t>Goode</t>
         </is>
       </c>
     </row>
@@ -550,7 +550,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Tryce</t>
+          <t>Blake</t>
         </is>
       </c>
     </row>
@@ -582,7 +582,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Schofield</t>
+          <t>Tanner</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Tryce</t>
         </is>
       </c>
     </row>
@@ -678,7 +678,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Noah</t>
+          <t>Hernandez</t>
         </is>
       </c>
     </row>
@@ -710,7 +710,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Hurley</t>
+          <t>Ben</t>
         </is>
       </c>
     </row>
@@ -742,7 +742,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Jaxson</t>
+          <t>Sidney</t>
         </is>
       </c>
     </row>
@@ -774,7 +774,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Jerzey</t>
+          <t>Riley</t>
         </is>
       </c>
     </row>
@@ -806,7 +806,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Kaleb</t>
+          <t>Nathan</t>
         </is>
       </c>
     </row>
@@ -838,7 +838,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Tommy</t>
+          <t>Noah</t>
         </is>
       </c>
     </row>
@@ -924,7 +924,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Garrett</t>
+          <t>Goode</t>
         </is>
       </c>
     </row>
@@ -956,7 +956,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Tryce</t>
+          <t>Aaron</t>
         </is>
       </c>
     </row>
@@ -988,7 +988,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Blake</t>
+          <t>Ben</t>
         </is>
       </c>
     </row>
@@ -1020,7 +1020,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Tryce</t>
+          <t>Blake</t>
         </is>
       </c>
     </row>
@@ -1052,7 +1052,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Creason</t>
+          <t>Hurley</t>
         </is>
       </c>
     </row>
@@ -1084,7 +1084,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Trey</t>
+          <t>Garrett</t>
         </is>
       </c>
     </row>
@@ -1200,7 +1200,7 @@
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Hurley</t>
+          <t>Garrett</t>
         </is>
       </c>
     </row>
@@ -1232,7 +1232,7 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Hurley</t>
+          <t>Blake</t>
         </is>
       </c>
     </row>
@@ -1264,7 +1264,7 @@
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Peyton</t>
+          <t>Aaron</t>
         </is>
       </c>
     </row>
@@ -1296,7 +1296,7 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Blake</t>
+          <t>EvanV</t>
         </is>
       </c>
     </row>
@@ -1328,7 +1328,7 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Garrett</t>
+          <t>Peyton</t>
         </is>
       </c>
     </row>
@@ -1476,7 +1476,7 @@
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Blake</t>
+          <t>Tryce</t>
         </is>
       </c>
     </row>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>EvanV</t>
+          <t>Peyton</t>
         </is>
       </c>
     </row>
@@ -1540,7 +1540,7 @@
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Goode</t>
+          <t>EvanV</t>
         </is>
       </c>
     </row>
@@ -1572,7 +1572,7 @@
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Aaron</t>
+          <t>Riley</t>
         </is>
       </c>
     </row>
@@ -1604,7 +1604,7 @@
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Landon</t>
+          <t>Garrett</t>
         </is>
       </c>
     </row>
@@ -1636,7 +1636,7 @@
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Garrett</t>
+          <t>Blake</t>
         </is>
       </c>
     </row>

</xml_diff>